<commit_message>
Removed Setup template from CardList.xlsx since it's not feasible to make generate with that template
</commit_message>
<xml_diff>
--- a/assets/CardList.xlsx
+++ b/assets/CardList.xlsx
@@ -5,13 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Guild" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Vox" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Lore" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Setup" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -78,42 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Player – Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symbol-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symbol-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symbol-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Player – Test</t>
   </si>
 </sst>
 </file>
@@ -33582,8 +33545,8 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38645,82 +38608,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.56"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>